<commit_message>
RestAPI Testing Code updated
</commit_message>
<xml_diff>
--- a/src/TestData/ExcelData/TestData.xlsx
+++ b/src/TestData/ExcelData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -51,16 +51,16 @@
     <t>ManulifeLaunchURLTest</t>
   </si>
   <si>
+    <t>Do Not Execute this Script.</t>
+  </si>
+  <si>
+    <t>Execute this Script.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>No</t>
-  </si>
-  <si>
-    <t>Do Not Execute this Script.</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Execute this Script.</t>
   </si>
 </sst>
 </file>
@@ -143,7 +143,7 @@
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -483,7 +483,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -494,13 +494,13 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTML - UI Base Design Prepared
</commit_message>
<xml_diff>
--- a/src/TestData/ExcelData/TestData.xlsx
+++ b/src/TestData/ExcelData/TestData.xlsx
@@ -2,21 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="TC_Details" r:id="rId1" sheetId="1"/>
-    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
-    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
+    <sheet name="TC_Details" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -55,19 +55,12 @@
   </si>
   <si>
     <t>Execute this Script.</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -135,21 +128,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -158,10 +151,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -317,7 +310,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -326,13 +319,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -342,7 +335,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -351,7 +344,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -360,7 +353,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -370,12 +363,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -406,7 +399,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -425,7 +418,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -438,7 +431,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C3"/>
@@ -446,10 +439,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -476,9 +469,7 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
@@ -493,9 +484,7 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
+      <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
@@ -504,7 +493,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -516,7 +505,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -528,6 +517,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LogFactory log implemented with xml log configuration
</commit_message>
<xml_diff>
--- a/src/TestData/ExcelData/TestData.xlsx
+++ b/src/TestData/ExcelData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>Execute this Script.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -469,7 +475,9 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
@@ -484,7 +492,9 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Script execution via Springboot configured and working
</commit_message>
<xml_diff>
--- a/src/TestData/ExcelData/TestData.xlsx
+++ b/src/TestData/ExcelData/TestData.xlsx
@@ -2,27 +2,21 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="TC_Details" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TC_Details" r:id="rId1" sheetId="1"/>
+    <sheet name="Sheet2" r:id="rId2" sheetId="2"/>
+    <sheet name="Sheet3" r:id="rId3" sheetId="3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
-  <si>
-    <t>TestCaseID</t>
-  </si>
-  <si>
-    <t>TestCaseName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>Execute_Flag</t>
   </si>
@@ -30,18 +24,6 @@
     <t>AutomationScriptName</t>
   </si>
   <si>
-    <t>testcase1</t>
-  </si>
-  <si>
-    <t>testcase2</t>
-  </si>
-  <si>
-    <t>firsttestcase</t>
-  </si>
-  <si>
-    <t>secondtestcase</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -58,15 +40,13 @@
   </si>
   <si>
     <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -134,21 +114,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -157,10 +136,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -316,7 +295,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -325,13 +304,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -341,7 +320,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -350,7 +329,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -359,7 +338,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,12 +348,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -405,7 +384,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -424,7 +403,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -437,73 +416,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="4" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -515,7 +474,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -527,6 +486,6 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>